<commit_message>
Add Text File [practice_typing]
</commit_message>
<xml_diff>
--- a/practice_typing.xlsx
+++ b/practice_typing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\김지혁\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3D0D894-AD4E-4677-883F-90BFBA99257D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC5A92A7-3961-474F-817E-8F4F6D2C1CCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="540" yWindow="975" windowWidth="16935" windowHeight="13680" xr2:uid="{113D0C04-CC4B-4748-B481-962982009824}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="49">
   <si>
     <t>자리연습</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -166,6 +166,62 @@
   </si>
   <si>
     <t>6분 10초</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1분 19초</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1분 4초</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1분</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1분 11초*</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1분 16초</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전날보다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3분 1초</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3분 31초</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4분 4초</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4분 30초</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4분 25초</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3분 43초</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>빨라짐</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>느려짐</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -193,7 +249,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -218,6 +274,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="12">
     <border>
@@ -350,7 +418,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -412,6 +480,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -731,20 +817,36 @@
   <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="I12" sqref="I11:I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="3" width="9" style="1"/>
-    <col min="4" max="5" width="9.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9" style="1"/>
+    <col min="4" max="6" width="9.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D1" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="3"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="F2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" s="21"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D3" s="2">
@@ -753,6 +855,9 @@
       <c r="E3" s="2">
         <v>44400</v>
       </c>
+      <c r="F3" s="2">
+        <v>44401</v>
+      </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -768,7 +873,9 @@
       <c r="E4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="5"/>
+      <c r="F4" s="22" t="s">
+        <v>35</v>
+      </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
@@ -789,7 +896,9 @@
       <c r="E5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="8"/>
+      <c r="F5" s="25" t="s">
+        <v>36</v>
+      </c>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
@@ -810,7 +919,9 @@
       <c r="E6" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="8"/>
+      <c r="F6" s="23" t="s">
+        <v>10</v>
+      </c>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
@@ -831,7 +942,9 @@
       <c r="E7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="8"/>
+      <c r="F7" s="25" t="s">
+        <v>37</v>
+      </c>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
@@ -852,7 +965,9 @@
       <c r="E8" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="8"/>
+      <c r="F8" s="25" t="s">
+        <v>36</v>
+      </c>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
@@ -873,7 +988,9 @@
       <c r="E9" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="8"/>
+      <c r="F9" s="24" t="s">
+        <v>38</v>
+      </c>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
@@ -894,7 +1011,9 @@
       <c r="E10" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="8"/>
+      <c r="F10" s="24" t="s">
+        <v>38</v>
+      </c>
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
@@ -915,7 +1034,9 @@
       <c r="E11" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="8"/>
+      <c r="F11" s="23" t="s">
+        <v>39</v>
+      </c>
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
       <c r="I11" s="8"/>
@@ -942,7 +1063,9 @@
       <c r="E12" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F12" s="8"/>
+      <c r="F12" s="25" t="s">
+        <v>41</v>
+      </c>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
@@ -961,7 +1084,9 @@
       <c r="E13" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="F13" s="8"/>
+      <c r="F13" s="25" t="s">
+        <v>42</v>
+      </c>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
       <c r="I13" s="8"/>
@@ -980,7 +1105,9 @@
       <c r="E14" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F14" s="8"/>
+      <c r="F14" s="25" t="s">
+        <v>43</v>
+      </c>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
@@ -999,7 +1126,9 @@
       <c r="E15" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="F15" s="8"/>
+      <c r="F15" s="25" t="s">
+        <v>44</v>
+      </c>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
       <c r="I15" s="8"/>
@@ -1018,7 +1147,9 @@
       <c r="E16" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="F16" s="8"/>
+      <c r="F16" s="25" t="s">
+        <v>44</v>
+      </c>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
       <c r="I16" s="8"/>
@@ -1037,7 +1168,9 @@
       <c r="E17" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F17" s="8"/>
+      <c r="F17" s="25" t="s">
+        <v>45</v>
+      </c>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
       <c r="I17" s="8"/>
@@ -1056,7 +1189,9 @@
       <c r="E18" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="F18" s="8"/>
+      <c r="F18" s="25" t="s">
+        <v>27</v>
+      </c>
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
       <c r="I18" s="8"/>
@@ -1075,7 +1210,9 @@
       <c r="E19" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="F19" s="12"/>
+      <c r="F19" s="26" t="s">
+        <v>46</v>
+      </c>
       <c r="G19" s="12"/>
       <c r="H19" s="12"/>
       <c r="I19" s="12"/>

</xml_diff>